<commit_message>
Add played games data and update portfolio content
Added a new playedgame.yml data file listing played games. Updated index.html to remove the tech stack colgroup and an interests description. Modified script.js to always use dark theme by default. Updated an Excel file and removed a PDF from the portfolio directory.
</commit_message>
<xml_diff>
--- a/portfolio/게임 플레이 리스트.xlsx
+++ b/portfolio/게임 플레이 리스트.xlsx
@@ -1645,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add two blog posts and update portfolio spreadsheet
Added two new markdown posts sharing game design thoughts and PM experiences related to League of Legends. Updated the portfolio Excel file with new data.
</commit_message>
<xml_diff>
--- a/portfolio/게임 플레이 리스트.xlsx
+++ b/portfolio/게임 플레이 리스트.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3af8901e2087a2c/GitHub Repository/hojun313.github.io/portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{8A090313-58BB-4B01-A26E-64F681B921A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2259FECA-00F7-459A-9306-B59B349E6E4E}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{8A090313-58BB-4B01-A26E-64F681B921A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E2E0CB9-C187-42F1-9516-66E4D1B251BA}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="17415" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,34 +129,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sid Meier's Civilization V</t>
-  </si>
-  <si>
     <t>150+</t>
   </si>
   <si>
-    <t>Terraria</t>
-  </si>
-  <si>
-    <t>Bubble Fighter</t>
-  </si>
-  <si>
     <t>100+</t>
-  </si>
-  <si>
-    <t>Cookie Clicker</t>
-  </si>
-  <si>
-    <t>Cookie Run: Kingdom</t>
-  </si>
-  <si>
-    <t>GTA5</t>
-  </si>
-  <si>
-    <t>Maple Story</t>
-  </si>
-  <si>
-    <t>Modoo Marble</t>
   </si>
   <si>
     <t>Palworld</t>
@@ -879,6 +855,38 @@
   </si>
   <si>
     <t>49 lvl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sid Meier's Civilization V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Terraria</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bubble Fighter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cookie Clicker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cookie Run: Kingdom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GTA5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Maple Story</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Modoo Marble</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1374,10 +1382,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1646,7 +1650,7 @@
   <dimension ref="A1:D187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A20" sqref="A20:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1701,7 +1705,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -1725,7 +1729,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -1737,7 +1741,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -1749,7 +1753,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -1791,463 +1795,463 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" s="15" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>29</v>
+        <v>257</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>30</v>
+        <v>258</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>32</v>
+        <v>259</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>31</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>39</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>33</v>
+        <v>260</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>34</v>
+        <v>261</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>39</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>35</v>
+        <v>262</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>36</v>
+        <v>263</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C24" s="17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C31" s="21"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C32" s="22"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C36" s="16"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="18" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C39" s="23"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C41" s="21"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="18" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C42" s="21"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="18" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C45" s="24" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="19" t="s">
         <v>86</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="18" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="18" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="18" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C52" s="16"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="25" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>10</v>
@@ -2255,266 +2259,266 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="25" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="25" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C56" s="27"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="25" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C57" s="27"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="25" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="25" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C59" s="27"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C61" s="27"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="25" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C62" s="27"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="25" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="25" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="25" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C66" s="27"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="25" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C67" s="27"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C68" s="27"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="25" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C70" s="27"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="25" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C71" s="27"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="25" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C72" s="27"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="25" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C73" s="27"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C74" s="27"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="25" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C75" s="27"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="25" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="25" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C78" s="27"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C79" s="26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="25" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="28" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C81" s="29">
         <v>0.8</v>
@@ -2522,315 +2526,315 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="25" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C82" s="27"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="25" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C83" s="26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="25" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C84" s="27"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="25" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="25" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="25" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C87" s="27"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="41" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="43"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="30" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C89" s="31"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="30" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C90" s="31"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="30" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C91" s="31"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="30" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C92" s="31"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="30" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C93" s="31"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="30" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C94" s="31"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="30" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C95" s="31"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="30" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C96" s="31"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="30" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C97" s="31"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="30" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C98" s="32" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="30" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C99" s="31"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="30" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C100" s="31"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="30" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C101" s="31"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="30" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C102" s="31"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="30" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C103" s="31"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="30" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C104" s="31"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="30" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C105" s="31"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="30" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C106" s="31"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="30" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C107" s="31"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="30" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="30" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C109" s="31"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="41" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B110" s="42"/>
       <c r="C110" s="43"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="33" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C111" s="34" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="33" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C112" s="27"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="33" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C113" s="27"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="33" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C114" s="27"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="33" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C115" s="34">
         <v>0.4</v>
@@ -2838,173 +2842,173 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="33" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C116" s="27"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="33" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C117" s="35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="33" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C118" s="35" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="33" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C119" s="27"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="33" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C120" s="27"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="33" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C121" s="35" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="33" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C122" s="27"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="33" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C123" s="27"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="33" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C124" s="27"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="33" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C125" s="27"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="33" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C126" s="27"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="33" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B127" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C127" s="27"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="33" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C128" s="27"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="33" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C129" s="35" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="33" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B130" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C130" s="27"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="33" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C131" s="27"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="33" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C132" s="35" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="33" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C133" s="36">
         <v>0.75</v>
@@ -3012,133 +3016,133 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="33" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C134" s="27"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="33" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C135" s="35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="33" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C136" s="27"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="33" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C137" s="27"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="33" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C138" s="27"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="33" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C139" s="27"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="33" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C140" s="27"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="33" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C141" s="27"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="33" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C142" s="27"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="33" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C143" s="27"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="33" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C144" s="35" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="33" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C145" s="35" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="33" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C146" s="27"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="33" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C147" s="34">
         <v>0.5</v>
@@ -3146,326 +3150,326 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="33" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C148" s="27"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="33" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C149" s="27"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="33" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C150" s="27"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="33" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C151" s="27"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="33" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C152" s="27"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="33" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C153" s="27"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="33" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C154" s="27"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="33" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C155" s="27"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="33" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C156" s="27"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="33" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C157" s="27"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="33" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C158" s="27"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="33" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C159" s="35" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="33" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C160" s="27"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="33" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B161" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C161" s="27"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="33" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B162" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C162" s="27"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="33" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B163" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C163" s="27"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="33" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B164" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C164" s="27"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="33" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C165" s="27"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="33" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B166" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C166" s="35" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="33" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B167" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C167" s="27"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="33" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B168" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C168" s="27"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="33" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B169" s="10" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C169" s="35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="33" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B170" s="10" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C170" s="27"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="33" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C171" s="27"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="33" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C172" s="27"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="33" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B173" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C173" s="27"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="33" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B174" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C174" s="27"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="33" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B175" s="10" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C175" s="35" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="33" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B176" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C176" s="27"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="33" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B177" s="10" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="33" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B178" s="10" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C178" s="27"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="33" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B179" s="10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C179" s="27"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="33" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B180" s="10" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C180" s="35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="33" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C181" s="27"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="33" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B182" s="10" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C182" s="40">
         <v>0.7</v>
@@ -3473,48 +3477,48 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="33" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B183" s="10" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C183" s="35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="33" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B184" s="10" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C184" s="27"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="33" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B185" s="10" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C185" s="27"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="33" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C186" s="27"/>
     </row>
     <row r="187" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A187" s="37" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B187" s="38" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C187" s="39"/>
     </row>

</xml_diff>